<commit_message>
update DataSource from webset
</commit_message>
<xml_diff>
--- a/Data source/Israel data/免疫指数相关/疫苗接种者在总人口中所占的百分比-按时间.xlsx
+++ b/Data source/Israel data/免疫指数相关/疫苗接种者在总人口中所占的百分比-按时间.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="17920" windowHeight="16520"/>
+    <workbookView windowWidth="17920" windowHeight="16380"/>
   </bookViews>
   <sheets>
     <sheet name="אחוז מתחסנים מכלל האוכלוסיה..." sheetId="1" r:id="rId1"/>
@@ -419,35 +419,13 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -467,8 +445,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -483,16 +507,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -509,14 +539,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -524,15 +546,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -547,7 +561,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -555,21 +569,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -584,6 +584,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -596,13 +602,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,25 +728,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -644,79 +746,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,43 +764,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -781,8 +781,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -811,6 +811,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -822,6 +846,17 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -840,186 +875,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1411,13 +1411,14 @@
   <dimension ref="A1:C130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="17.6" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="38.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="17.3571428571429" customWidth="1"/>
+    <col min="3" max="3" width="22.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2848,7 +2849,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="A3:C130 B1:C1" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:C1 A3:C130" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>